<commit_message>
Hopefully finally fix for databank issue...
</commit_message>
<xml_diff>
--- a/data/Physioswiss Stellen Historisch 22012024-test.xlsx
+++ b/data/Physioswiss Stellen Historisch 22012024-test.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="315">
   <si>
     <t>Arbeitgeber</t>
   </si>
@@ -84,13 +84,895 @@
   </si>
   <si>
     <t>Aktiv</t>
+  </si>
+  <si>
+    <t>Fitness &amp; Physio Zentrum First GmbH</t>
+  </si>
+  <si>
+    <t>Gesundheitspraxis Löwen Center AG</t>
+  </si>
+  <si>
+    <t>Gesundheitszentrum Allschwil AG</t>
+  </si>
+  <si>
+    <t>Kantonsspital Aarau</t>
+  </si>
+  <si>
+    <t>Lindenhofgruppe AG</t>
+  </si>
+  <si>
+    <t>Medbase Wil</t>
+  </si>
+  <si>
+    <t>Myophysio</t>
+  </si>
+  <si>
+    <t>PHYSIOZONE AG</t>
+  </si>
+  <si>
+    <t>Physio DÄHLER</t>
+  </si>
+  <si>
+    <t>Physio Halter</t>
+  </si>
+  <si>
+    <t>Physiokandil GmbH</t>
+  </si>
+  <si>
+    <t>Physiotherapie Giessen</t>
+  </si>
+  <si>
+    <t>Physiotherapie Kipfgasse-Buchsi GmbH</t>
+  </si>
+  <si>
+    <t>Physiozentrum – Solothurn</t>
+  </si>
+  <si>
+    <t>Physiozentrum – Wil</t>
+  </si>
+  <si>
+    <t>Physiozentrum – Winterthur</t>
+  </si>
+  <si>
+    <t>Regionalspital Emmental AG</t>
+  </si>
+  <si>
+    <t>Réseau Santé Balcon du Jura.vd</t>
+  </si>
+  <si>
+    <t>STUDIO-11 LLC</t>
+  </si>
+  <si>
+    <t>SYNERGY Fitness + Physio</t>
+  </si>
+  <si>
+    <t>Saluto AG</t>
+  </si>
+  <si>
+    <t>Spital Bülach AG</t>
+  </si>
+  <si>
+    <t>Spital Uster</t>
+  </si>
+  <si>
+    <t>Stiftung Scalottas</t>
+  </si>
+  <si>
+    <t>UNIVERSITÄRE PSYCHIATRISCHE DIENSTE BERN (UPD) AG</t>
+  </si>
+  <si>
+    <t>Zuger Kantonsspital AG</t>
+  </si>
+  <si>
+    <t>Firststrasse 31</t>
+  </si>
+  <si>
+    <t>Zürichstr. 9</t>
+  </si>
+  <si>
+    <t>Baslerstrasse 126</t>
+  </si>
+  <si>
+    <t>Tellstrasse 25</t>
+  </si>
+  <si>
+    <t>Muristr. 12</t>
+  </si>
+  <si>
+    <t>Friedtalweg 18</t>
+  </si>
+  <si>
+    <t>Im Hag 11</t>
+  </si>
+  <si>
+    <t>Müligässli 1</t>
+  </si>
+  <si>
+    <t>Place de la gare 8</t>
+  </si>
+  <si>
+    <t>Mülhauserstrasse 70</t>
+  </si>
+  <si>
+    <t>Hardstrase 221</t>
+  </si>
+  <si>
+    <t>Giessenplatz 1</t>
+  </si>
+  <si>
+    <t>Kipfgasse 7 und Schöneggweg 1a</t>
+  </si>
+  <si>
+    <t>Dorchnacherstrasse 28/28a</t>
+  </si>
+  <si>
+    <t>Obere Bahnhofstrasse 26</t>
+  </si>
+  <si>
+    <t>Bahnhofplatz 8</t>
+  </si>
+  <si>
+    <t>Oberburgstrasse 54</t>
+  </si>
+  <si>
+    <t>Rue des Rosiers 29</t>
+  </si>
+  <si>
+    <t>7 Rue Maunoir</t>
+  </si>
+  <si>
+    <t>Burgdorfstrasse 36</t>
+  </si>
+  <si>
+    <t>Chli Ebnet 3</t>
+  </si>
+  <si>
+    <t>Spitalstrasse 24</t>
+  </si>
+  <si>
+    <t>Brunnenstrasse 42</t>
+  </si>
+  <si>
+    <t>Carutta 2</t>
+  </si>
+  <si>
+    <t>Bolligenstrasse 111</t>
+  </si>
+  <si>
+    <t>Landhausstrasse 11</t>
+  </si>
+  <si>
+    <t>Physiotherapie</t>
+  </si>
+  <si>
+    <t>HRM</t>
+  </si>
+  <si>
+    <t>8835</t>
+  </si>
+  <si>
+    <t>6004</t>
+  </si>
+  <si>
+    <t>4123</t>
+  </si>
+  <si>
+    <t>5000</t>
+  </si>
+  <si>
+    <t>3001</t>
+  </si>
+  <si>
+    <t>9500</t>
+  </si>
+  <si>
+    <t>5033</t>
+  </si>
+  <si>
+    <t>8598</t>
+  </si>
+  <si>
+    <t>1740</t>
+  </si>
+  <si>
+    <t>4056</t>
+  </si>
+  <si>
+    <t>8005</t>
+  </si>
+  <si>
+    <t>8600</t>
+  </si>
+  <si>
+    <t>3053</t>
+  </si>
+  <si>
+    <t>4500</t>
+  </si>
+  <si>
+    <t>8400</t>
+  </si>
+  <si>
+    <t>3400</t>
+  </si>
+  <si>
+    <t>1450</t>
+  </si>
+  <si>
+    <t>1207</t>
+  </si>
+  <si>
+    <t>3672</t>
+  </si>
+  <si>
+    <t>6403</t>
+  </si>
+  <si>
+    <t>8180</t>
+  </si>
+  <si>
+    <t>8610</t>
+  </si>
+  <si>
+    <t>7412</t>
+  </si>
+  <si>
+    <t>3000</t>
+  </si>
+  <si>
+    <t>6340</t>
+  </si>
+  <si>
+    <t>Feusisberg</t>
+  </si>
+  <si>
+    <t>Luzern</t>
+  </si>
+  <si>
+    <t>Allschwil</t>
+  </si>
+  <si>
+    <t>Aarau</t>
+  </si>
+  <si>
+    <t>Bern</t>
+  </si>
+  <si>
+    <t>Wil</t>
+  </si>
+  <si>
+    <t>Buchs</t>
+  </si>
+  <si>
+    <t>Bottighofen</t>
+  </si>
+  <si>
+    <t>Neyruz</t>
+  </si>
+  <si>
+    <t>Basel</t>
+  </si>
+  <si>
+    <t>Zürich</t>
+  </si>
+  <si>
+    <t>Dübendorf</t>
+  </si>
+  <si>
+    <t>Münchenbuchsee</t>
+  </si>
+  <si>
+    <t>Solothurn</t>
+  </si>
+  <si>
+    <t>Winterthur</t>
+  </si>
+  <si>
+    <t>Burgdorf</t>
+  </si>
+  <si>
+    <t>Sainte-Croix</t>
+  </si>
+  <si>
+    <t>Genève</t>
+  </si>
+  <si>
+    <t>Oberdiessbach</t>
+  </si>
+  <si>
+    <t>Küssnacht</t>
+  </si>
+  <si>
+    <t>Bülach</t>
+  </si>
+  <si>
+    <t>Uster</t>
+  </si>
+  <si>
+    <t>Scharans</t>
+  </si>
+  <si>
+    <t>Baar</t>
+  </si>
+  <si>
+    <t>Schwyz</t>
+  </si>
+  <si>
+    <t>Basel-Landschaft</t>
+  </si>
+  <si>
+    <t>Aargau</t>
+  </si>
+  <si>
+    <t>St. Gallen</t>
+  </si>
+  <si>
+    <t>Thurgau</t>
+  </si>
+  <si>
+    <t>Freiburg</t>
+  </si>
+  <si>
+    <t>Basel-Stadt</t>
+  </si>
+  <si>
+    <t>Waadt</t>
+  </si>
+  <si>
+    <t>Genf</t>
+  </si>
+  <si>
+    <t>Graubünden</t>
+  </si>
+  <si>
+    <t>Zug</t>
+  </si>
+  <si>
+    <t>Zurich</t>
+  </si>
+  <si>
+    <t>Geneve</t>
+  </si>
+  <si>
+    <t>Ja</t>
+  </si>
+  <si>
+    <t>Aufgestellte Physiotherapeuten Raum oberer Zürichsee</t>
+  </si>
+  <si>
+    <t>Dipl. Physiotherapeut/In FH/HF 40-100%</t>
+  </si>
+  <si>
+    <t>Physiotherapeut:In für 50%-100%</t>
+  </si>
+  <si>
+    <t>Dipl. Physiotherapeut/in Pädiatrie 50-100%</t>
+  </si>
+  <si>
+    <t>Dipl. Physiotherapeut/in 50 - 100 %</t>
+  </si>
+  <si>
+    <t>Physiotherapeut (w/m/d) 40% - 100%</t>
+  </si>
+  <si>
+    <t>Physiotherapeut/in 20-100% in Buchs AG in Umsatzbeteiligung</t>
+  </si>
+  <si>
+    <t>Dipl. Physiotherapeut/in 60 - 100%</t>
+  </si>
+  <si>
+    <t>Deux physiothérapeutes 60-100 % (salarié/ indépendant)</t>
+  </si>
+  <si>
+    <t>Ciao, Lust auf ein tolles Team?</t>
+  </si>
+  <si>
+    <t>dipl. Physiotherapeut/in FH (40-100%)</t>
+  </si>
+  <si>
+    <t>Physiotherapeut:in 10 - 100% in Höngg Zürich</t>
+  </si>
+  <si>
+    <t>dipl. Physiotherapeut*in 30-80%</t>
+  </si>
+  <si>
+    <t>PhysiotherapeutIn (40-100%) für Zentrum in Solothurn gesucht</t>
+  </si>
+  <si>
+    <t>Domizil-PhysiotherapeutIn (40-100%) für Wil gesucht</t>
+  </si>
+  <si>
+    <t>PhysiotherapeutIn (40 - 100%) für Zentrum in Winterthur gesucht</t>
+  </si>
+  <si>
+    <t>dipl. Physiotherapeut:in 60-100% Burgdorf + Langnau</t>
+  </si>
+  <si>
+    <t>Physiothérapeute 80 à 100%</t>
+  </si>
+  <si>
+    <t>Physiothérapeute H/F dans un centre sportif</t>
+  </si>
+  <si>
+    <t>Dipl. Physiotherapeut/in</t>
+  </si>
+  <si>
+    <t>Dipl. (Sport-)Physiotherapeut:in (60 - 100%)</t>
+  </si>
+  <si>
+    <t>Physiotherapeutin/Physiotherapeut 70 - 90 %</t>
+  </si>
+  <si>
+    <t>Physiotherapeut*in HF/FH 90%</t>
+  </si>
+  <si>
+    <t>Physiotherapeut:in</t>
+  </si>
+  <si>
+    <t>Dipl. Physiotherapeut FH / HF (w/m/d)</t>
+  </si>
+  <si>
+    <t>Physiotherapeutin</t>
+  </si>
+  <si>
+    <t>60 - 100 %</t>
+  </si>
+  <si>
+    <t>40 - 100 %</t>
+  </si>
+  <si>
+    <t>50 - 100 %</t>
+  </si>
+  <si>
+    <t>20 - 100 %</t>
+  </si>
+  <si>
+    <t>60 - 80 %</t>
+  </si>
+  <si>
+    <t>10 - 100 %</t>
+  </si>
+  <si>
+    <t>30 - 80 %</t>
+  </si>
+  <si>
+    <t>80 - 100 %</t>
+  </si>
+  <si>
+    <t>70 - 90 %</t>
+  </si>
+  <si>
+    <t>90 %</t>
+  </si>
+  <si>
+    <t>80 %</t>
+  </si>
+  <si>
+    <t>60 %</t>
+  </si>
+  <si>
+    <t>Nach Vereinbarung</t>
+  </si>
+  <si>
+    <t>Sofort</t>
+  </si>
+  <si>
+    <t>Freitag, 1. März 2024</t>
+  </si>
+  <si>
+    <t>Donnerstag, 1. Februar 2024</t>
+  </si>
+  <si>
+    <t>Donnerstag, 2. Mai 2024</t>
+  </si>
+  <si>
+    <t>Festanstellung</t>
+  </si>
+  <si>
+    <t>Stundenlohn</t>
+  </si>
+  <si>
+    <t>20-12-2023</t>
+  </si>
+  <si>
+    <t>21-12-2023</t>
+  </si>
+  <si>
+    <t>22-12-2023</t>
+  </si>
+  <si>
+    <t>17-01-2024</t>
+  </si>
+  <si>
+    <t>20-11-2023</t>
+  </si>
+  <si>
+    <t>07-01-2024</t>
+  </si>
+  <si>
+    <t>01-01-2024</t>
+  </si>
+  <si>
+    <t>09-01-2024</t>
+  </si>
+  <si>
+    <t>16-01-2024</t>
+  </si>
+  <si>
+    <t>22-01-2024</t>
+  </si>
+  <si>
+    <t>Herr Philipp oder Andreas Engler</t>
+  </si>
+  <si>
+    <t>Frau José van der Hoef</t>
+  </si>
+  <si>
+    <t>Frau Cornelia Graf Cardinale</t>
+  </si>
+  <si>
+    <t>Frau Nadine Schärmeli</t>
+  </si>
+  <si>
+    <t>Frau Suzanne Christen</t>
+  </si>
+  <si>
+    <t>Herr Christoph Beyer</t>
+  </si>
+  <si>
+    <t>Herr Mario Muilwijk</t>
+  </si>
+  <si>
+    <t>Frau Dunja Späth</t>
+  </si>
+  <si>
+    <t>Frau Barbara Dähler</t>
+  </si>
+  <si>
+    <t>Herr Gene Halter</t>
+  </si>
+  <si>
+    <t>Herr Tamim Kandil</t>
+  </si>
+  <si>
+    <t>Herr Carlo Paganoni</t>
+  </si>
+  <si>
+    <t>Frau Catherine Dohnal</t>
+  </si>
+  <si>
+    <t>Frau Martina Landolt</t>
+  </si>
+  <si>
+    <t>Frau Kristina Manzke</t>
+  </si>
+  <si>
+    <t>Herr Jérémy Zonca</t>
+  </si>
+  <si>
+    <t>Herr Baptiste Chalot</t>
+  </si>
+  <si>
+    <t>Herr MAS Martin Weichmann</t>
+  </si>
+  <si>
+    <t>Frau Linda Bürgi</t>
+  </si>
+  <si>
+    <t>Frau Corinne von Gunten</t>
+  </si>
+  <si>
+    <t>Herr Marcel Ambass</t>
+  </si>
+  <si>
+    <t>Frau Mirjam Vincenz</t>
+  </si>
+  <si>
+    <t>Frau - Recruiting</t>
+  </si>
+  <si>
+    <t>Herr Serge Wilhelm</t>
+  </si>
+  <si>
+    <t>0435365039</t>
+  </si>
+  <si>
+    <t>0414106940</t>
+  </si>
+  <si>
+    <t>0614859393</t>
+  </si>
+  <si>
+    <t>0041628384944</t>
+  </si>
+  <si>
+    <t>0041313008017</t>
+  </si>
+  <si>
+    <t>0719135490</t>
+  </si>
+  <si>
+    <t>0766678857</t>
+  </si>
+  <si>
+    <t>0715714065</t>
+  </si>
+  <si>
+    <t>0762976197</t>
+  </si>
+  <si>
+    <t>0442123800</t>
+  </si>
+  <si>
+    <t>0762125313</t>
+  </si>
+  <si>
+    <t>0442713368</t>
+  </si>
+  <si>
+    <t>0344212253</t>
+  </si>
+  <si>
+    <t>0244551642</t>
+  </si>
+  <si>
+    <t>0317713020</t>
+  </si>
+  <si>
+    <t>0418504365</t>
+  </si>
+  <si>
+    <t>0041448632224</t>
+  </si>
+  <si>
+    <t>0449111190</t>
+  </si>
+  <si>
+    <t>0816321818</t>
+  </si>
+  <si>
+    <t>0041319309429</t>
+  </si>
+  <si>
+    <t>0413994470</t>
+  </si>
+  <si>
+    <t>0782199908</t>
+  </si>
+  <si>
+    <t>0792388699</t>
+  </si>
+  <si>
+    <t>0789750011</t>
+  </si>
+  <si>
+    <t>info@fitness-physio-first.ch</t>
+  </si>
+  <si>
+    <t>info@physio-luzern.ch</t>
+  </si>
+  <si>
+    <t>physiogza@hin.ch</t>
+  </si>
+  <si>
+    <t>bewerbung@ksa.ch</t>
+  </si>
+  <si>
+    <t>hrm@lindenhofgruppe.ch</t>
+  </si>
+  <si>
+    <t>christoph.beyer@medbase.ch</t>
+  </si>
+  <si>
+    <t>info@myophysio.ch</t>
+  </si>
+  <si>
+    <t>home@physiozone.ch</t>
+  </si>
+  <si>
+    <t>barbara@physio-daehler.ch</t>
+  </si>
+  <si>
+    <t>info@physio-halter.ch</t>
+  </si>
+  <si>
+    <t>info@physiokandil.ch</t>
+  </si>
+  <si>
+    <t>jobs@physiotherapie-giessen.ch</t>
+  </si>
+  <si>
+    <t>cdohnal@physiokipfgasse.ch</t>
+  </si>
+  <si>
+    <t>jobs@physiozentrum.ch</t>
+  </si>
+  <si>
+    <t>kristina.manzke@spital-emmental.ch</t>
+  </si>
+  <si>
+    <t>jeremy.zonca@rsbj.ch</t>
+  </si>
+  <si>
+    <t>contact@studio-11.ch</t>
+  </si>
+  <si>
+    <t>info@phys-io.ch</t>
+  </si>
+  <si>
+    <t>info@saluto.ch</t>
+  </si>
+  <si>
+    <t>bewerbung@scalottas.ch</t>
+  </si>
+  <si>
+    <t>bewerbungen@upd.ch</t>
+  </si>
+  <si>
+    <t>personal@zgks.ch</t>
+  </si>
+  <si>
+    <t>http://fitness-physio-first.ch/</t>
+  </si>
+  <si>
+    <t>http://www.physio-luzern.ch/</t>
+  </si>
+  <si>
+    <t>https://www.gesund-in-allschwil.ch/</t>
+  </si>
+  <si>
+    <t>https://www.ksa.ch/</t>
+  </si>
+  <si>
+    <t>https://www.lindenhofgruppe.ch/de/</t>
+  </si>
+  <si>
+    <t>https://www.medicosearch.ch/medbase-wil-friedtalweg-18-9500-wil/surgery/35245</t>
+  </si>
+  <si>
+    <t>https://myophysio.ch/</t>
+  </si>
+  <si>
+    <t>http://www.physiozone.ch/</t>
+  </si>
+  <si>
+    <t>http://www.physio-daehler.ch/</t>
+  </si>
+  <si>
+    <t>https://www.physio-halter.ch/</t>
+  </si>
+  <si>
+    <t>http://physiokandil.ch/</t>
+  </si>
+  <si>
+    <t>http://www.physiotherapie-giessen.ch/</t>
+  </si>
+  <si>
+    <t>http://www.physiokipfgasse.ch/</t>
+  </si>
+  <si>
+    <t>http://www.physiozentrum.ch/solothurn</t>
+  </si>
+  <si>
+    <t>https://www.physiozentrum.ch/wil/</t>
+  </si>
+  <si>
+    <t>http://www.physiozentrum.ch/winterthur/</t>
+  </si>
+  <si>
+    <t>https://www.spital-emmental.ch/</t>
+  </si>
+  <si>
+    <t>https://www.rsbj.ch/</t>
+  </si>
+  <si>
+    <t>http://www.studio-11.ch/</t>
+  </si>
+  <si>
+    <t>http://www.phys-io.ch/</t>
+  </si>
+  <si>
+    <t>https://www.saluto.ch/</t>
+  </si>
+  <si>
+    <t>https://www.spitalbuelach.ch/</t>
+  </si>
+  <si>
+    <t>https://www.spitaluster.ch/</t>
+  </si>
+  <si>
+    <t>http://www.scalottas.ch/</t>
+  </si>
+  <si>
+    <t>https://www.upd.ch/de/</t>
+  </si>
+  <si>
+    <t>http://www.zgks.ch/</t>
+  </si>
+  <si>
+    <t>https://www.physioswiss.ch/de/jobs/246432/aufgestellte-physiotherapeuten-raum-oberer-zuerichsee</t>
+  </si>
+  <si>
+    <t>https://www.physioswiss.ch/de/jobs/246487/dipl-physiotherapeut-in-fh-hf-40-100</t>
+  </si>
+  <si>
+    <t>https://www.physioswiss.ch/de/jobs/243825/physiotherapeut-in-fuer-50-100</t>
+  </si>
+  <si>
+    <t>https://www.physioswiss.ch/de/jobs/246410/dipl-physiotherapeut-in-paediatrie-50-100</t>
+  </si>
+  <si>
+    <t>https://www.physioswiss.ch/de/jobs/246475/dipl-physiotherapeut-in-50-100</t>
+  </si>
+  <si>
+    <t>https://www.physioswiss.ch/de/jobs/246429/physiotherapeut-w-m-d-40-100</t>
+  </si>
+  <si>
+    <t>https://www.physioswiss.ch/de/jobs/247856/physiotherapeut-in-20-100-in-buchs-ag-in-umsatzbeteiligung</t>
+  </si>
+  <si>
+    <t>https://www.physioswiss.ch/de/jobs/246456/dipl-physiotherapeut-in-60-100</t>
+  </si>
+  <si>
+    <t>https://www.physioswiss.ch/de/jobs/244514/deux-physiotherapeutes-60-100-salarie-independant</t>
+  </si>
+  <si>
+    <t>https://www.physioswiss.ch/de/jobs/246574/ciao-lust-auf-ein-tolles-team</t>
+  </si>
+  <si>
+    <t>https://www.physioswiss.ch/de/jobs/246439/dipl-physiotherapeut-in-fh-40-100</t>
+  </si>
+  <si>
+    <t>https://www.physioswiss.ch/de/jobs/246588/physiotherapeut-in-10-100-in-hoengg-zuerich</t>
+  </si>
+  <si>
+    <t>https://www.physioswiss.ch/de/jobs/247009/dipl-physiotherapeut-in-30-80</t>
+  </si>
+  <si>
+    <t>https://www.physioswiss.ch/de/jobs/246533/physiotherapeutin-40-100-fuer-zentrum-in-solothurn-gesucht</t>
+  </si>
+  <si>
+    <t>https://www.physioswiss.ch/de/jobs/244811/domizil-physiotherapeutin-40-100-fuer-wil-gesucht</t>
+  </si>
+  <si>
+    <t>https://www.physioswiss.ch/de/jobs/246464/physiotherapeutin-40-100-fuer-zentrum-in-winterthur-gesucht</t>
+  </si>
+  <si>
+    <t>https://www.physioswiss.ch/de/jobs/246263/dipl-physiotherapeut-in-60-100-burgdorf-langnau</t>
+  </si>
+  <si>
+    <t>https://www.physioswiss.ch/de/jobs/246466/physiotherapeute-80-a-100</t>
+  </si>
+  <si>
+    <t>https://www.physioswiss.ch/de/jobs/246388/physiotherapeute-h-f-dans-un-centre-sportif</t>
+  </si>
+  <si>
+    <t>https://www.physioswiss.ch/de/jobs/246452/dipl-physiotherapeut-in</t>
+  </si>
+  <si>
+    <t>https://www.physioswiss.ch/de/jobs/246557/dipl-sport-physiotherapeut-in-60-100</t>
+  </si>
+  <si>
+    <t>https://www.physioswiss.ch/de/jobs/246473/physiotherapeutin-physiotherapeut-70-90</t>
+  </si>
+  <si>
+    <t>https://www.physioswiss.ch/de/jobs/246485/physiotherapeut-in-hf-fh-90</t>
+  </si>
+  <si>
+    <t>https://www.physioswiss.ch/de/jobs/247123/physiotherapeut-in</t>
+  </si>
+  <si>
+    <t>https://www.physioswiss.ch/de/jobs/247766/dipl-physiotherapeut-fh-hf-w-m-d</t>
+  </si>
+  <si>
+    <t>https://www.physioswiss.ch/de/jobs/246575/physiotherapeutin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,6 +987,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -139,16 +1028,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -441,7 +1336,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:U27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -512,14 +1407,1455 @@
         <v>20</v>
       </c>
     </row>
+    <row r="2" spans="1:21">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" t="s">
+        <v>124</v>
+      </c>
+      <c r="I2" t="s">
+        <v>138</v>
+      </c>
+      <c r="J2" t="s">
+        <v>164</v>
+      </c>
+      <c r="K2" t="s">
+        <v>176</v>
+      </c>
+      <c r="L2" t="s">
+        <v>181</v>
+      </c>
+      <c r="M2" t="s">
+        <v>183</v>
+      </c>
+      <c r="N2" t="s">
+        <v>192</v>
+      </c>
+      <c r="O2" t="s">
+        <v>193</v>
+      </c>
+      <c r="P2" t="s">
+        <v>217</v>
+      </c>
+      <c r="R2" t="s">
+        <v>241</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G3" t="s">
+        <v>101</v>
+      </c>
+      <c r="H3" t="s">
+        <v>137</v>
+      </c>
+      <c r="I3" t="s">
+        <v>139</v>
+      </c>
+      <c r="J3" t="s">
+        <v>165</v>
+      </c>
+      <c r="K3" t="s">
+        <v>176</v>
+      </c>
+      <c r="L3" t="s">
+        <v>181</v>
+      </c>
+      <c r="M3" t="s">
+        <v>184</v>
+      </c>
+      <c r="N3" t="s">
+        <v>192</v>
+      </c>
+      <c r="O3" t="s">
+        <v>194</v>
+      </c>
+      <c r="P3" t="s">
+        <v>218</v>
+      </c>
+      <c r="R3" t="s">
+        <v>242</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G4" t="s">
+        <v>109</v>
+      </c>
+      <c r="I4" t="s">
+        <v>140</v>
+      </c>
+      <c r="J4" t="s">
+        <v>166</v>
+      </c>
+      <c r="K4" t="s">
+        <v>176</v>
+      </c>
+      <c r="L4" t="s">
+        <v>181</v>
+      </c>
+      <c r="M4" t="s">
+        <v>185</v>
+      </c>
+      <c r="N4" t="s">
+        <v>192</v>
+      </c>
+      <c r="O4" t="s">
+        <v>195</v>
+      </c>
+      <c r="P4" t="s">
+        <v>219</v>
+      </c>
+      <c r="R4" t="s">
+        <v>243</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F5" t="s">
+        <v>126</v>
+      </c>
+      <c r="I5" t="s">
+        <v>141</v>
+      </c>
+      <c r="J5" t="s">
+        <v>166</v>
+      </c>
+      <c r="K5" t="s">
+        <v>176</v>
+      </c>
+      <c r="L5" t="s">
+        <v>181</v>
+      </c>
+      <c r="M5" t="s">
+        <v>183</v>
+      </c>
+      <c r="N5" t="s">
+        <v>192</v>
+      </c>
+      <c r="O5" t="s">
+        <v>196</v>
+      </c>
+      <c r="P5" t="s">
+        <v>220</v>
+      </c>
+      <c r="R5" t="s">
+        <v>244</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F6" t="s">
+        <v>104</v>
+      </c>
+      <c r="G6" t="s">
+        <v>104</v>
+      </c>
+      <c r="I6" t="s">
+        <v>142</v>
+      </c>
+      <c r="J6" t="s">
+        <v>166</v>
+      </c>
+      <c r="K6" t="s">
+        <v>177</v>
+      </c>
+      <c r="L6" t="s">
+        <v>181</v>
+      </c>
+      <c r="M6" t="s">
+        <v>184</v>
+      </c>
+      <c r="N6" t="s">
+        <v>192</v>
+      </c>
+      <c r="O6" t="s">
+        <v>197</v>
+      </c>
+      <c r="P6" t="s">
+        <v>221</v>
+      </c>
+      <c r="R6" t="s">
+        <v>245</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I7" t="s">
+        <v>143</v>
+      </c>
+      <c r="J7" t="s">
+        <v>165</v>
+      </c>
+      <c r="K7" t="s">
+        <v>177</v>
+      </c>
+      <c r="L7" t="s">
+        <v>181</v>
+      </c>
+      <c r="M7" t="s">
+        <v>183</v>
+      </c>
+      <c r="N7" t="s">
+        <v>192</v>
+      </c>
+      <c r="O7" t="s">
+        <v>198</v>
+      </c>
+      <c r="P7" t="s">
+        <v>222</v>
+      </c>
+      <c r="R7" t="s">
+        <v>246</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" t="s">
+        <v>126</v>
+      </c>
+      <c r="H8" t="s">
+        <v>137</v>
+      </c>
+      <c r="I8" t="s">
+        <v>144</v>
+      </c>
+      <c r="J8" t="s">
+        <v>167</v>
+      </c>
+      <c r="K8" t="s">
+        <v>176</v>
+      </c>
+      <c r="L8" t="s">
+        <v>182</v>
+      </c>
+      <c r="M8" t="s">
+        <v>186</v>
+      </c>
+      <c r="N8" t="s">
+        <v>192</v>
+      </c>
+      <c r="O8" t="s">
+        <v>199</v>
+      </c>
+      <c r="P8" t="s">
+        <v>223</v>
+      </c>
+      <c r="R8" t="s">
+        <v>247</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F9" t="s">
+        <v>128</v>
+      </c>
+      <c r="H9" t="s">
+        <v>137</v>
+      </c>
+      <c r="I9" t="s">
+        <v>145</v>
+      </c>
+      <c r="J9" t="s">
+        <v>164</v>
+      </c>
+      <c r="K9" t="s">
+        <v>176</v>
+      </c>
+      <c r="L9" t="s">
+        <v>181</v>
+      </c>
+      <c r="M9" t="s">
+        <v>185</v>
+      </c>
+      <c r="N9" t="s">
+        <v>192</v>
+      </c>
+      <c r="O9" t="s">
+        <v>200</v>
+      </c>
+      <c r="P9" t="s">
+        <v>224</v>
+      </c>
+      <c r="R9" t="s">
+        <v>248</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="T9" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" t="s">
+        <v>108</v>
+      </c>
+      <c r="F10" t="s">
+        <v>129</v>
+      </c>
+      <c r="I10" t="s">
+        <v>146</v>
+      </c>
+      <c r="J10" t="s">
+        <v>164</v>
+      </c>
+      <c r="K10" t="s">
+        <v>176</v>
+      </c>
+      <c r="L10" t="s">
+        <v>181</v>
+      </c>
+      <c r="M10" t="s">
+        <v>187</v>
+      </c>
+      <c r="N10" t="s">
+        <v>192</v>
+      </c>
+      <c r="O10" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>238</v>
+      </c>
+      <c r="R10" t="s">
+        <v>249</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" t="s">
+        <v>109</v>
+      </c>
+      <c r="F11" t="s">
+        <v>130</v>
+      </c>
+      <c r="G11" t="s">
+        <v>109</v>
+      </c>
+      <c r="H11" t="s">
+        <v>137</v>
+      </c>
+      <c r="I11" t="s">
+        <v>147</v>
+      </c>
+      <c r="J11" t="s">
+        <v>168</v>
+      </c>
+      <c r="K11" t="s">
+        <v>176</v>
+      </c>
+      <c r="L11" t="s">
+        <v>181</v>
+      </c>
+      <c r="M11" t="s">
+        <v>185</v>
+      </c>
+      <c r="N11" t="s">
+        <v>192</v>
+      </c>
+      <c r="O11" t="s">
+        <v>202</v>
+      </c>
+      <c r="P11" t="s">
+        <v>225</v>
+      </c>
+      <c r="R11" t="s">
+        <v>250</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E12" t="s">
+        <v>110</v>
+      </c>
+      <c r="F12" t="s">
+        <v>110</v>
+      </c>
+      <c r="G12" t="s">
+        <v>135</v>
+      </c>
+      <c r="I12" t="s">
+        <v>148</v>
+      </c>
+      <c r="J12" t="s">
+        <v>165</v>
+      </c>
+      <c r="K12" t="s">
+        <v>178</v>
+      </c>
+      <c r="L12" t="s">
+        <v>181</v>
+      </c>
+      <c r="M12" t="s">
+        <v>183</v>
+      </c>
+      <c r="N12" t="s">
+        <v>192</v>
+      </c>
+      <c r="O12" t="s">
+        <v>203</v>
+      </c>
+      <c r="P12" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>226</v>
+      </c>
+      <c r="R12" t="s">
+        <v>251</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" t="s">
+        <v>111</v>
+      </c>
+      <c r="F13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G13" t="s">
+        <v>135</v>
+      </c>
+      <c r="H13" t="s">
+        <v>137</v>
+      </c>
+      <c r="I13" t="s">
+        <v>149</v>
+      </c>
+      <c r="J13" t="s">
+        <v>169</v>
+      </c>
+      <c r="K13" t="s">
+        <v>176</v>
+      </c>
+      <c r="L13" t="s">
+        <v>181</v>
+      </c>
+      <c r="M13" t="s">
+        <v>185</v>
+      </c>
+      <c r="N13" t="s">
+        <v>192</v>
+      </c>
+      <c r="O13" t="s">
+        <v>204</v>
+      </c>
+      <c r="P13" t="s">
+        <v>227</v>
+      </c>
+      <c r="R13" t="s">
+        <v>252</v>
+      </c>
+      <c r="S13" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="T13" s="2" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" t="s">
+        <v>87</v>
+      </c>
+      <c r="E14" t="s">
+        <v>112</v>
+      </c>
+      <c r="F14" t="s">
+        <v>104</v>
+      </c>
+      <c r="G14" t="s">
+        <v>104</v>
+      </c>
+      <c r="H14" t="s">
+        <v>137</v>
+      </c>
+      <c r="I14" t="s">
+        <v>150</v>
+      </c>
+      <c r="J14" t="s">
+        <v>170</v>
+      </c>
+      <c r="K14" t="s">
+        <v>176</v>
+      </c>
+      <c r="L14" t="s">
+        <v>181</v>
+      </c>
+      <c r="M14" t="s">
+        <v>188</v>
+      </c>
+      <c r="N14" t="s">
+        <v>192</v>
+      </c>
+      <c r="O14" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>239</v>
+      </c>
+      <c r="R14" t="s">
+        <v>253</v>
+      </c>
+      <c r="S14" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="T14" s="2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" t="s">
+        <v>113</v>
+      </c>
+      <c r="F15" t="s">
+        <v>113</v>
+      </c>
+      <c r="H15" t="s">
+        <v>137</v>
+      </c>
+      <c r="I15" t="s">
+        <v>151</v>
+      </c>
+      <c r="J15" t="s">
+        <v>165</v>
+      </c>
+      <c r="K15" t="s">
+        <v>179</v>
+      </c>
+      <c r="L15" t="s">
+        <v>181</v>
+      </c>
+      <c r="M15" t="s">
+        <v>189</v>
+      </c>
+      <c r="N15" t="s">
+        <v>192</v>
+      </c>
+      <c r="O15" t="s">
+        <v>206</v>
+      </c>
+      <c r="P15" t="s">
+        <v>228</v>
+      </c>
+      <c r="R15" t="s">
+        <v>254</v>
+      </c>
+      <c r="S15" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="T15" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" t="s">
+        <v>105</v>
+      </c>
+      <c r="F16" t="s">
+        <v>127</v>
+      </c>
+      <c r="H16" t="s">
+        <v>137</v>
+      </c>
+      <c r="I16" t="s">
+        <v>152</v>
+      </c>
+      <c r="J16" t="s">
+        <v>165</v>
+      </c>
+      <c r="K16" t="s">
+        <v>177</v>
+      </c>
+      <c r="L16" t="s">
+        <v>181</v>
+      </c>
+      <c r="M16" t="s">
+        <v>185</v>
+      </c>
+      <c r="N16" t="s">
+        <v>192</v>
+      </c>
+      <c r="O16" t="s">
+        <v>206</v>
+      </c>
+      <c r="P16" t="s">
+        <v>228</v>
+      </c>
+      <c r="R16" t="s">
+        <v>254</v>
+      </c>
+      <c r="S16" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="T16" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" t="s">
+        <v>114</v>
+      </c>
+      <c r="F17" t="s">
+        <v>110</v>
+      </c>
+      <c r="G17" t="s">
+        <v>135</v>
+      </c>
+      <c r="H17" t="s">
+        <v>137</v>
+      </c>
+      <c r="I17" t="s">
+        <v>153</v>
+      </c>
+      <c r="J17" t="s">
+        <v>165</v>
+      </c>
+      <c r="K17" t="s">
+        <v>180</v>
+      </c>
+      <c r="L17" t="s">
+        <v>181</v>
+      </c>
+      <c r="M17" t="s">
+        <v>183</v>
+      </c>
+      <c r="N17" t="s">
+        <v>192</v>
+      </c>
+      <c r="O17" t="s">
+        <v>206</v>
+      </c>
+      <c r="P17" t="s">
+        <v>228</v>
+      </c>
+      <c r="R17" t="s">
+        <v>254</v>
+      </c>
+      <c r="S17" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="T17" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" t="s">
+        <v>115</v>
+      </c>
+      <c r="F18" t="s">
+        <v>104</v>
+      </c>
+      <c r="G18" t="s">
+        <v>104</v>
+      </c>
+      <c r="I18" t="s">
+        <v>154</v>
+      </c>
+      <c r="J18" t="s">
+        <v>164</v>
+      </c>
+      <c r="K18" t="s">
+        <v>176</v>
+      </c>
+      <c r="L18" t="s">
+        <v>181</v>
+      </c>
+      <c r="M18" t="s">
+        <v>185</v>
+      </c>
+      <c r="N18" t="s">
+        <v>192</v>
+      </c>
+      <c r="O18" t="s">
+        <v>207</v>
+      </c>
+      <c r="P18" t="s">
+        <v>229</v>
+      </c>
+      <c r="R18" t="s">
+        <v>255</v>
+      </c>
+      <c r="S18" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="T18" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E19" t="s">
+        <v>116</v>
+      </c>
+      <c r="F19" t="s">
+        <v>131</v>
+      </c>
+      <c r="I19" t="s">
+        <v>155</v>
+      </c>
+      <c r="J19" t="s">
+        <v>171</v>
+      </c>
+      <c r="K19" t="s">
+        <v>177</v>
+      </c>
+      <c r="L19" t="s">
+        <v>181</v>
+      </c>
+      <c r="M19" t="s">
+        <v>183</v>
+      </c>
+      <c r="N19" t="s">
+        <v>192</v>
+      </c>
+      <c r="O19" t="s">
+        <v>208</v>
+      </c>
+      <c r="P19" t="s">
+        <v>230</v>
+      </c>
+      <c r="R19" t="s">
+        <v>256</v>
+      </c>
+      <c r="S19" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="T19" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20" t="s">
+        <v>117</v>
+      </c>
+      <c r="F20" t="s">
+        <v>132</v>
+      </c>
+      <c r="G20" t="s">
+        <v>136</v>
+      </c>
+      <c r="I20" t="s">
+        <v>156</v>
+      </c>
+      <c r="J20" t="s">
+        <v>166</v>
+      </c>
+      <c r="K20" t="s">
+        <v>176</v>
+      </c>
+      <c r="L20" t="s">
+        <v>181</v>
+      </c>
+      <c r="M20" t="s">
+        <v>183</v>
+      </c>
+      <c r="N20" t="s">
+        <v>192</v>
+      </c>
+      <c r="O20" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>240</v>
+      </c>
+      <c r="R20" t="s">
+        <v>257</v>
+      </c>
+      <c r="S20" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="T20" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" t="s">
+        <v>93</v>
+      </c>
+      <c r="E21" t="s">
+        <v>118</v>
+      </c>
+      <c r="F21" t="s">
+        <v>104</v>
+      </c>
+      <c r="G21" t="s">
+        <v>104</v>
+      </c>
+      <c r="H21" t="s">
+        <v>137</v>
+      </c>
+      <c r="I21" t="s">
+        <v>157</v>
+      </c>
+      <c r="J21" t="s">
+        <v>166</v>
+      </c>
+      <c r="K21" t="s">
+        <v>176</v>
+      </c>
+      <c r="L21" t="s">
+        <v>181</v>
+      </c>
+      <c r="M21" t="s">
+        <v>183</v>
+      </c>
+      <c r="N21" t="s">
+        <v>192</v>
+      </c>
+      <c r="O21" t="s">
+        <v>210</v>
+      </c>
+      <c r="P21" t="s">
+        <v>231</v>
+      </c>
+      <c r="R21" t="s">
+        <v>258</v>
+      </c>
+      <c r="S21" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="T21" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" t="s">
+        <v>94</v>
+      </c>
+      <c r="E22" t="s">
+        <v>119</v>
+      </c>
+      <c r="F22" t="s">
+        <v>124</v>
+      </c>
+      <c r="G22" t="s">
+        <v>101</v>
+      </c>
+      <c r="I22" t="s">
+        <v>158</v>
+      </c>
+      <c r="J22" t="s">
+        <v>164</v>
+      </c>
+      <c r="K22" t="s">
+        <v>177</v>
+      </c>
+      <c r="L22" t="s">
+        <v>181</v>
+      </c>
+      <c r="M22" t="s">
+        <v>185</v>
+      </c>
+      <c r="N22" t="s">
+        <v>192</v>
+      </c>
+      <c r="O22" t="s">
+        <v>211</v>
+      </c>
+      <c r="P22" t="s">
+        <v>232</v>
+      </c>
+      <c r="R22" t="s">
+        <v>259</v>
+      </c>
+      <c r="S22" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="T22" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20">
+      <c r="A23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" t="s">
+        <v>95</v>
+      </c>
+      <c r="E23" t="s">
+        <v>120</v>
+      </c>
+      <c r="F23" t="s">
+        <v>110</v>
+      </c>
+      <c r="G23" t="s">
+        <v>135</v>
+      </c>
+      <c r="I23" t="s">
+        <v>159</v>
+      </c>
+      <c r="J23" t="s">
+        <v>172</v>
+      </c>
+      <c r="K23" t="s">
+        <v>179</v>
+      </c>
+      <c r="L23" t="s">
+        <v>181</v>
+      </c>
+      <c r="M23" t="s">
+        <v>184</v>
+      </c>
+      <c r="N23" t="s">
+        <v>192</v>
+      </c>
+      <c r="O23" t="s">
+        <v>212</v>
+      </c>
+      <c r="P23" t="s">
+        <v>233</v>
+      </c>
+      <c r="S23" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="T23" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20">
+      <c r="A24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" t="s">
+        <v>96</v>
+      </c>
+      <c r="E24" t="s">
+        <v>121</v>
+      </c>
+      <c r="F24" t="s">
+        <v>110</v>
+      </c>
+      <c r="G24" t="s">
+        <v>135</v>
+      </c>
+      <c r="I24" t="s">
+        <v>160</v>
+      </c>
+      <c r="J24" t="s">
+        <v>173</v>
+      </c>
+      <c r="K24" t="s">
+        <v>177</v>
+      </c>
+      <c r="L24" t="s">
+        <v>181</v>
+      </c>
+      <c r="M24" t="s">
+        <v>184</v>
+      </c>
+      <c r="N24" t="s">
+        <v>192</v>
+      </c>
+      <c r="O24" t="s">
+        <v>213</v>
+      </c>
+      <c r="P24" t="s">
+        <v>234</v>
+      </c>
+      <c r="S24" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="T24" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20">
+      <c r="A25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" t="s">
+        <v>97</v>
+      </c>
+      <c r="E25" t="s">
+        <v>122</v>
+      </c>
+      <c r="F25" t="s">
+        <v>133</v>
+      </c>
+      <c r="I25" t="s">
+        <v>161</v>
+      </c>
+      <c r="J25" t="s">
+        <v>174</v>
+      </c>
+      <c r="K25" t="s">
+        <v>176</v>
+      </c>
+      <c r="L25" t="s">
+        <v>181</v>
+      </c>
+      <c r="M25" t="s">
+        <v>190</v>
+      </c>
+      <c r="N25" t="s">
+        <v>192</v>
+      </c>
+      <c r="O25" t="s">
+        <v>214</v>
+      </c>
+      <c r="P25" t="s">
+        <v>235</v>
+      </c>
+      <c r="R25" t="s">
+        <v>260</v>
+      </c>
+      <c r="S25" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="T25" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="A26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" t="s">
+        <v>98</v>
+      </c>
+      <c r="E26" t="s">
+        <v>104</v>
+      </c>
+      <c r="F26" t="s">
+        <v>104</v>
+      </c>
+      <c r="G26" t="s">
+        <v>104</v>
+      </c>
+      <c r="I26" t="s">
+        <v>162</v>
+      </c>
+      <c r="J26" t="s">
+        <v>175</v>
+      </c>
+      <c r="K26" t="s">
+        <v>178</v>
+      </c>
+      <c r="L26" t="s">
+        <v>181</v>
+      </c>
+      <c r="M26" t="s">
+        <v>191</v>
+      </c>
+      <c r="N26" t="s">
+        <v>192</v>
+      </c>
+      <c r="O26" t="s">
+        <v>215</v>
+      </c>
+      <c r="P26" t="s">
+        <v>236</v>
+      </c>
+      <c r="R26" t="s">
+        <v>261</v>
+      </c>
+      <c r="S26" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="T26" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20">
+      <c r="A27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" t="s">
+        <v>99</v>
+      </c>
+      <c r="E27" t="s">
+        <v>123</v>
+      </c>
+      <c r="F27" t="s">
+        <v>134</v>
+      </c>
+      <c r="G27" t="s">
+        <v>101</v>
+      </c>
+      <c r="H27" t="s">
+        <v>137</v>
+      </c>
+      <c r="I27" t="s">
+        <v>163</v>
+      </c>
+      <c r="J27" t="s">
+        <v>166</v>
+      </c>
+      <c r="K27" t="s">
+        <v>176</v>
+      </c>
+      <c r="L27" t="s">
+        <v>181</v>
+      </c>
+      <c r="M27" t="s">
+        <v>185</v>
+      </c>
+      <c r="N27" t="s">
+        <v>192</v>
+      </c>
+      <c r="O27" t="s">
+        <v>216</v>
+      </c>
+      <c r="P27" t="s">
+        <v>237</v>
+      </c>
+      <c r="R27" t="s">
+        <v>262</v>
+      </c>
+      <c r="S27" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="T27" s="2" t="s">
+        <v>314</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="S2" r:id="rId1"/>
+    <hyperlink ref="T2" r:id="rId2"/>
+    <hyperlink ref="S3" r:id="rId3"/>
+    <hyperlink ref="T3" r:id="rId4"/>
+    <hyperlink ref="S4" r:id="rId5"/>
+    <hyperlink ref="T4" r:id="rId6"/>
+    <hyperlink ref="S5" r:id="rId7"/>
+    <hyperlink ref="T5" r:id="rId8"/>
+    <hyperlink ref="S6" r:id="rId9"/>
+    <hyperlink ref="T6" r:id="rId10"/>
+    <hyperlink ref="S7" r:id="rId11"/>
+    <hyperlink ref="T7" r:id="rId12"/>
+    <hyperlink ref="S8" r:id="rId13"/>
+    <hyperlink ref="T8" r:id="rId14"/>
+    <hyperlink ref="S9" r:id="rId15"/>
+    <hyperlink ref="T9" r:id="rId16"/>
+    <hyperlink ref="S10" r:id="rId17"/>
+    <hyperlink ref="T10" r:id="rId18"/>
+    <hyperlink ref="S11" r:id="rId19"/>
+    <hyperlink ref="T11" r:id="rId20"/>
+    <hyperlink ref="S12" r:id="rId21"/>
+    <hyperlink ref="T12" r:id="rId22"/>
+    <hyperlink ref="S13" r:id="rId23"/>
+    <hyperlink ref="T13" r:id="rId24"/>
+    <hyperlink ref="S14" r:id="rId25"/>
+    <hyperlink ref="T14" r:id="rId26"/>
+    <hyperlink ref="S15" r:id="rId27"/>
+    <hyperlink ref="T15" r:id="rId28"/>
+    <hyperlink ref="S16" r:id="rId29"/>
+    <hyperlink ref="T16" r:id="rId30"/>
+    <hyperlink ref="S17" r:id="rId31"/>
+    <hyperlink ref="T17" r:id="rId32"/>
+    <hyperlink ref="S18" r:id="rId33"/>
+    <hyperlink ref="T18" r:id="rId34"/>
+    <hyperlink ref="S19" r:id="rId35"/>
+    <hyperlink ref="T19" r:id="rId36"/>
+    <hyperlink ref="S20" r:id="rId37"/>
+    <hyperlink ref="T20" r:id="rId38"/>
+    <hyperlink ref="S21" r:id="rId39"/>
+    <hyperlink ref="T21" r:id="rId40"/>
+    <hyperlink ref="S22" r:id="rId41"/>
+    <hyperlink ref="T22" r:id="rId42"/>
+    <hyperlink ref="S23" r:id="rId43"/>
+    <hyperlink ref="T23" r:id="rId44"/>
+    <hyperlink ref="S24" r:id="rId45"/>
+    <hyperlink ref="T24" r:id="rId46"/>
+    <hyperlink ref="S25" r:id="rId47"/>
+    <hyperlink ref="T25" r:id="rId48"/>
+    <hyperlink ref="S26" r:id="rId49"/>
+    <hyperlink ref="T26" r:id="rId50"/>
+    <hyperlink ref="S27" r:id="rId51"/>
+    <hyperlink ref="T27" r:id="rId52"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -590,14 +2926,132 @@
         <v>20</v>
       </c>
     </row>
+    <row r="2" spans="1:21">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G2" t="s">
+        <v>109</v>
+      </c>
+      <c r="I2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J2" t="s">
+        <v>166</v>
+      </c>
+      <c r="K2" t="s">
+        <v>176</v>
+      </c>
+      <c r="L2" t="s">
+        <v>181</v>
+      </c>
+      <c r="M2" t="s">
+        <v>185</v>
+      </c>
+      <c r="N2" t="s">
+        <v>192</v>
+      </c>
+      <c r="O2" t="s">
+        <v>195</v>
+      </c>
+      <c r="P2" t="s">
+        <v>219</v>
+      </c>
+      <c r="R2" t="s">
+        <v>243</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F3" t="s">
+        <v>130</v>
+      </c>
+      <c r="G3" t="s">
+        <v>109</v>
+      </c>
+      <c r="H3" t="s">
+        <v>137</v>
+      </c>
+      <c r="I3" t="s">
+        <v>147</v>
+      </c>
+      <c r="J3" t="s">
+        <v>168</v>
+      </c>
+      <c r="K3" t="s">
+        <v>176</v>
+      </c>
+      <c r="L3" t="s">
+        <v>181</v>
+      </c>
+      <c r="M3" t="s">
+        <v>185</v>
+      </c>
+      <c r="N3" t="s">
+        <v>192</v>
+      </c>
+      <c r="O3" t="s">
+        <v>202</v>
+      </c>
+      <c r="P3" t="s">
+        <v>225</v>
+      </c>
+      <c r="R3" t="s">
+        <v>250</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="S2" r:id="rId1"/>
+    <hyperlink ref="T2" r:id="rId2"/>
+    <hyperlink ref="S3" r:id="rId3"/>
+    <hyperlink ref="T3" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -668,14 +3122,300 @@
         <v>20</v>
       </c>
     </row>
+    <row r="2" spans="1:21">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G2" t="s">
+        <v>104</v>
+      </c>
+      <c r="I2" t="s">
+        <v>142</v>
+      </c>
+      <c r="J2" t="s">
+        <v>166</v>
+      </c>
+      <c r="K2" t="s">
+        <v>177</v>
+      </c>
+      <c r="L2" t="s">
+        <v>181</v>
+      </c>
+      <c r="M2" t="s">
+        <v>184</v>
+      </c>
+      <c r="N2" t="s">
+        <v>192</v>
+      </c>
+      <c r="O2" t="s">
+        <v>197</v>
+      </c>
+      <c r="P2" t="s">
+        <v>221</v>
+      </c>
+      <c r="R2" t="s">
+        <v>245</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G3" t="s">
+        <v>104</v>
+      </c>
+      <c r="H3" t="s">
+        <v>137</v>
+      </c>
+      <c r="I3" t="s">
+        <v>150</v>
+      </c>
+      <c r="J3" t="s">
+        <v>170</v>
+      </c>
+      <c r="K3" t="s">
+        <v>176</v>
+      </c>
+      <c r="L3" t="s">
+        <v>181</v>
+      </c>
+      <c r="M3" t="s">
+        <v>188</v>
+      </c>
+      <c r="N3" t="s">
+        <v>192</v>
+      </c>
+      <c r="O3" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>239</v>
+      </c>
+      <c r="R3" t="s">
+        <v>253</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G4" t="s">
+        <v>104</v>
+      </c>
+      <c r="I4" t="s">
+        <v>154</v>
+      </c>
+      <c r="J4" t="s">
+        <v>164</v>
+      </c>
+      <c r="K4" t="s">
+        <v>176</v>
+      </c>
+      <c r="L4" t="s">
+        <v>181</v>
+      </c>
+      <c r="M4" t="s">
+        <v>185</v>
+      </c>
+      <c r="N4" t="s">
+        <v>192</v>
+      </c>
+      <c r="O4" t="s">
+        <v>207</v>
+      </c>
+      <c r="P4" t="s">
+        <v>229</v>
+      </c>
+      <c r="R4" t="s">
+        <v>255</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" t="s">
+        <v>118</v>
+      </c>
+      <c r="F5" t="s">
+        <v>104</v>
+      </c>
+      <c r="G5" t="s">
+        <v>104</v>
+      </c>
+      <c r="H5" t="s">
+        <v>137</v>
+      </c>
+      <c r="I5" t="s">
+        <v>157</v>
+      </c>
+      <c r="J5" t="s">
+        <v>166</v>
+      </c>
+      <c r="K5" t="s">
+        <v>176</v>
+      </c>
+      <c r="L5" t="s">
+        <v>181</v>
+      </c>
+      <c r="M5" t="s">
+        <v>183</v>
+      </c>
+      <c r="N5" t="s">
+        <v>192</v>
+      </c>
+      <c r="O5" t="s">
+        <v>210</v>
+      </c>
+      <c r="P5" t="s">
+        <v>231</v>
+      </c>
+      <c r="R5" t="s">
+        <v>258</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F6" t="s">
+        <v>104</v>
+      </c>
+      <c r="G6" t="s">
+        <v>104</v>
+      </c>
+      <c r="I6" t="s">
+        <v>162</v>
+      </c>
+      <c r="J6" t="s">
+        <v>175</v>
+      </c>
+      <c r="K6" t="s">
+        <v>178</v>
+      </c>
+      <c r="L6" t="s">
+        <v>181</v>
+      </c>
+      <c r="M6" t="s">
+        <v>191</v>
+      </c>
+      <c r="N6" t="s">
+        <v>192</v>
+      </c>
+      <c r="O6" t="s">
+        <v>215</v>
+      </c>
+      <c r="P6" t="s">
+        <v>236</v>
+      </c>
+      <c r="R6" t="s">
+        <v>261</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="S2" r:id="rId1"/>
+    <hyperlink ref="T2" r:id="rId2"/>
+    <hyperlink ref="S3" r:id="rId3"/>
+    <hyperlink ref="T3" r:id="rId4"/>
+    <hyperlink ref="S4" r:id="rId5"/>
+    <hyperlink ref="T4" r:id="rId6"/>
+    <hyperlink ref="S5" r:id="rId7"/>
+    <hyperlink ref="T5" r:id="rId8"/>
+    <hyperlink ref="S6" r:id="rId9"/>
+    <hyperlink ref="T6" r:id="rId10"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -746,7 +3486,64 @@
         <v>20</v>
       </c>
     </row>
+    <row r="2" spans="1:21">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G2" t="s">
+        <v>136</v>
+      </c>
+      <c r="I2" t="s">
+        <v>156</v>
+      </c>
+      <c r="J2" t="s">
+        <v>166</v>
+      </c>
+      <c r="K2" t="s">
+        <v>176</v>
+      </c>
+      <c r="L2" t="s">
+        <v>181</v>
+      </c>
+      <c r="M2" t="s">
+        <v>183</v>
+      </c>
+      <c r="N2" t="s">
+        <v>192</v>
+      </c>
+      <c r="O2" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>240</v>
+      </c>
+      <c r="R2" t="s">
+        <v>257</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="S2" r:id="rId1"/>
+    <hyperlink ref="T2" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -831,7 +3628,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -902,7 +3699,183 @@
         <v>20</v>
       </c>
     </row>
+    <row r="2" spans="1:21">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" t="s">
+        <v>137</v>
+      </c>
+      <c r="I2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J2" t="s">
+        <v>165</v>
+      </c>
+      <c r="K2" t="s">
+        <v>176</v>
+      </c>
+      <c r="L2" t="s">
+        <v>181</v>
+      </c>
+      <c r="M2" t="s">
+        <v>184</v>
+      </c>
+      <c r="N2" t="s">
+        <v>192</v>
+      </c>
+      <c r="O2" t="s">
+        <v>194</v>
+      </c>
+      <c r="P2" t="s">
+        <v>218</v>
+      </c>
+      <c r="R2" t="s">
+        <v>242</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" t="s">
+        <v>119</v>
+      </c>
+      <c r="F3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I3" t="s">
+        <v>158</v>
+      </c>
+      <c r="J3" t="s">
+        <v>164</v>
+      </c>
+      <c r="K3" t="s">
+        <v>177</v>
+      </c>
+      <c r="L3" t="s">
+        <v>181</v>
+      </c>
+      <c r="M3" t="s">
+        <v>185</v>
+      </c>
+      <c r="N3" t="s">
+        <v>192</v>
+      </c>
+      <c r="O3" t="s">
+        <v>211</v>
+      </c>
+      <c r="P3" t="s">
+        <v>232</v>
+      </c>
+      <c r="R3" t="s">
+        <v>259</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E4" t="s">
+        <v>123</v>
+      </c>
+      <c r="F4" t="s">
+        <v>134</v>
+      </c>
+      <c r="G4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H4" t="s">
+        <v>137</v>
+      </c>
+      <c r="I4" t="s">
+        <v>163</v>
+      </c>
+      <c r="J4" t="s">
+        <v>166</v>
+      </c>
+      <c r="K4" t="s">
+        <v>176</v>
+      </c>
+      <c r="L4" t="s">
+        <v>181</v>
+      </c>
+      <c r="M4" t="s">
+        <v>185</v>
+      </c>
+      <c r="N4" t="s">
+        <v>192</v>
+      </c>
+      <c r="O4" t="s">
+        <v>216</v>
+      </c>
+      <c r="P4" t="s">
+        <v>237</v>
+      </c>
+      <c r="R4" t="s">
+        <v>262</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>314</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="S2" r:id="rId1"/>
+    <hyperlink ref="T2" r:id="rId2"/>
+    <hyperlink ref="S3" r:id="rId3"/>
+    <hyperlink ref="T3" r:id="rId4"/>
+    <hyperlink ref="S4" r:id="rId5"/>
+    <hyperlink ref="T4" r:id="rId6"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -987,7 +3960,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1058,7 +4031,287 @@
         <v>20</v>
       </c>
     </row>
+    <row r="2" spans="1:21">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G2" t="s">
+        <v>135</v>
+      </c>
+      <c r="I2" t="s">
+        <v>148</v>
+      </c>
+      <c r="J2" t="s">
+        <v>165</v>
+      </c>
+      <c r="K2" t="s">
+        <v>178</v>
+      </c>
+      <c r="L2" t="s">
+        <v>181</v>
+      </c>
+      <c r="M2" t="s">
+        <v>183</v>
+      </c>
+      <c r="N2" t="s">
+        <v>192</v>
+      </c>
+      <c r="O2" t="s">
+        <v>203</v>
+      </c>
+      <c r="P2" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>226</v>
+      </c>
+      <c r="R2" t="s">
+        <v>251</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G3" t="s">
+        <v>135</v>
+      </c>
+      <c r="H3" t="s">
+        <v>137</v>
+      </c>
+      <c r="I3" t="s">
+        <v>149</v>
+      </c>
+      <c r="J3" t="s">
+        <v>169</v>
+      </c>
+      <c r="K3" t="s">
+        <v>176</v>
+      </c>
+      <c r="L3" t="s">
+        <v>181</v>
+      </c>
+      <c r="M3" t="s">
+        <v>185</v>
+      </c>
+      <c r="N3" t="s">
+        <v>192</v>
+      </c>
+      <c r="O3" t="s">
+        <v>204</v>
+      </c>
+      <c r="P3" t="s">
+        <v>227</v>
+      </c>
+      <c r="R3" t="s">
+        <v>252</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G4" t="s">
+        <v>135</v>
+      </c>
+      <c r="H4" t="s">
+        <v>137</v>
+      </c>
+      <c r="I4" t="s">
+        <v>153</v>
+      </c>
+      <c r="J4" t="s">
+        <v>165</v>
+      </c>
+      <c r="K4" t="s">
+        <v>180</v>
+      </c>
+      <c r="L4" t="s">
+        <v>181</v>
+      </c>
+      <c r="M4" t="s">
+        <v>183</v>
+      </c>
+      <c r="N4" t="s">
+        <v>192</v>
+      </c>
+      <c r="O4" t="s">
+        <v>206</v>
+      </c>
+      <c r="P4" t="s">
+        <v>228</v>
+      </c>
+      <c r="R4" t="s">
+        <v>254</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" t="s">
+        <v>120</v>
+      </c>
+      <c r="F5" t="s">
+        <v>110</v>
+      </c>
+      <c r="G5" t="s">
+        <v>135</v>
+      </c>
+      <c r="I5" t="s">
+        <v>159</v>
+      </c>
+      <c r="J5" t="s">
+        <v>172</v>
+      </c>
+      <c r="K5" t="s">
+        <v>179</v>
+      </c>
+      <c r="L5" t="s">
+        <v>181</v>
+      </c>
+      <c r="M5" t="s">
+        <v>184</v>
+      </c>
+      <c r="N5" t="s">
+        <v>192</v>
+      </c>
+      <c r="O5" t="s">
+        <v>212</v>
+      </c>
+      <c r="P5" t="s">
+        <v>233</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6" t="s">
+        <v>121</v>
+      </c>
+      <c r="F6" t="s">
+        <v>110</v>
+      </c>
+      <c r="G6" t="s">
+        <v>135</v>
+      </c>
+      <c r="I6" t="s">
+        <v>160</v>
+      </c>
+      <c r="J6" t="s">
+        <v>173</v>
+      </c>
+      <c r="K6" t="s">
+        <v>177</v>
+      </c>
+      <c r="L6" t="s">
+        <v>181</v>
+      </c>
+      <c r="M6" t="s">
+        <v>184</v>
+      </c>
+      <c r="N6" t="s">
+        <v>192</v>
+      </c>
+      <c r="O6" t="s">
+        <v>213</v>
+      </c>
+      <c r="P6" t="s">
+        <v>234</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="S2" r:id="rId1"/>
+    <hyperlink ref="T2" r:id="rId2"/>
+    <hyperlink ref="S3" r:id="rId3"/>
+    <hyperlink ref="T3" r:id="rId4"/>
+    <hyperlink ref="S4" r:id="rId5"/>
+    <hyperlink ref="T4" r:id="rId6"/>
+    <hyperlink ref="S5" r:id="rId7"/>
+    <hyperlink ref="T5" r:id="rId8"/>
+    <hyperlink ref="S6" r:id="rId9"/>
+    <hyperlink ref="T6" r:id="rId10"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>